<commit_message>
chore: add edge evaluation
</commit_message>
<xml_diff>
--- a/experiments/edge_results.xlsx
+++ b/experiments/edge_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qinsz\Desktop\NLP_project\03code\IDExtraction\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DB2559-3B89-45C0-B66C-0C9E2850E995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A99685B-2032-44F3-A8BC-122AEA1CFA7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9132" yWindow="5052" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>extraction_cot</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -61,6 +61,14 @@
   </si>
   <si>
     <t>edit_distance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>extraction_0shot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>generation_0shot</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -386,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -412,41 +420,57 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>2.6372550000000001</v>
+        <v>2.6764705882352939</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>2.4356435643564356</v>
+        <v>2.6372550000000001</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
-        <v>3.5145631067961167</v>
+        <v>2.4356435643564356</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>3.233009708737864</v>
+        <v>3.5145631067961167</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>3.3398058252427183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>3.233009708737864</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B9">
         <v>3.2524271844660193</v>
       </c>
     </row>

</xml_diff>